<commit_message>
Changed business names from YPS - Bridge Mobile Phils., Inc.
</commit_message>
<xml_diff>
--- a/Business Plan Documents/Breakeven_Analysis.xlsx
+++ b/Business Plan Documents/Breakeven_Analysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Z MINSYST - TENTREP\tentrep-yps\Business Plan Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5130"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="15345" windowHeight="5130"/>
   </bookViews>
   <sheets>
     <sheet name="Breakeven Analysis" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -302,22 +302,22 @@
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -338,7 +338,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -356,397 +356,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1025" name="Text Box 1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9601200" y="1095375"/>
-          <a:ext cx="1714500" cy="5238750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFF99" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="43"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="1" i="0" u="sng" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>Instructions</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>Note: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>You may want to print this information to use as reference later.  To delete these instructions, click the border of this text box and then press the DELETE key.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>Using figures from your Profit and Loss Projection, enter expected annual fixed and variable costs.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>Fixed costs are those that remain the same regardless of your sales volume. They are expressed in dollars. Rent, insurance and real estate taxes, for example, are usually fixed.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>Variable costs are those which change as your volume of business changes. They are expressed as a percent of sales. Inventory, raw materials and direct production labor, for example, are usually variable costs.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>For your business, each category of expense may either be fixed or variable, but not both.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="Text Box 2"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="57150" y="5943600"/>
-          <a:ext cx="4733925" cy="2228850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFF99" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="43"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="1" i="0" u="sng" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>Suggestions</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>Note:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t> You may want to print this information to use as reference later. To delete these instructions, click the border of this text box and then press the DELETE key.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>The categories of expense shown above are just suggestions. Change the labels to reflect your own accounting systems and type of business. Breakeven is a "big picture" kind of tool; we recommend that you combine expense categories to stay within the 22 lines that this template allows.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>One of the best uses of breakeven analysis is to play with various scenarios. For instance, if you add another person to the payroll, how many extra sales dollars will be needed to recover the extra salary expense? If you borrow, how much will be needed to cover the increased principal and interest payments? Many owners, especially retailers, like to calculate a daily breakdown. This gives everyone a target to shoot at for the day.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1017,8 +626,8 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1442,7 +1051,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="92" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>